<commit_message>
fix laporan tambah total dan terbilang
</commit_message>
<xml_diff>
--- a/contoh.xlsx
+++ b/contoh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\keuangan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89706A89-45F5-443B-9E9B-6935F7650C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44ECBE0C-E87D-4761-8B17-6112E6E53BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7270" xr2:uid="{38268120-CC6A-4F47-BED0-D63DDA726784}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7725" xr2:uid="{38268120-CC6A-4F47-BED0-D63DDA726784}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>nama</t>
   </si>
@@ -51,9 +51,6 @@
     <t>diterima</t>
   </si>
   <si>
-    <t>nik</t>
-  </si>
-  <si>
     <t>61002</t>
   </si>
   <si>
@@ -99,20 +96,17 @@
     <t>Nama Jabatan 5</t>
   </si>
   <si>
-    <t>tidak menggunakan rumus pada halaman excel ini !</t>
-  </si>
-  <si>
-    <t>PERHATIAN !</t>
-  </si>
-  <si>
     <t>kode_akses</t>
+  </si>
+  <si>
+    <t>nip/nrpk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,27 +120,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -161,14 +141,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,23 +458,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637E2570-28A3-46C7-945F-A28F6A7E4610}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.36328125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -517,123 +491,133 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>100000</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <f>2%*D2</f>
+        <v>2000</v>
       </c>
       <c r="F2">
-        <v>100000</v>
+        <f>D2-E2</f>
+        <v>98000</v>
       </c>
       <c r="G2">
         <v>12345</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>200000</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <f t="shared" ref="E3:E6" si="0">2%*D3</f>
+        <v>4000</v>
       </c>
       <c r="F3">
-        <v>200000</v>
+        <f t="shared" ref="F3:F6" si="1">D3-E3</f>
+        <v>196000</v>
       </c>
       <c r="G3">
-        <v>54321</v>
-      </c>
-      <c r="H3" s="2"/>
+        <v>12345</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>300000</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6000</v>
       </c>
       <c r="F4">
-        <v>300000</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>21</v>
+        <f t="shared" si="1"/>
+        <v>294000</v>
+      </c>
+      <c r="G4">
+        <v>12345</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>400000</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>8000</v>
       </c>
       <c r="F5">
-        <v>400000</v>
-      </c>
-      <c r="H5" s="3"/>
+        <f t="shared" si="1"/>
+        <v>392000</v>
+      </c>
+      <c r="G5">
+        <v>12345</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>500000</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>10000</v>
       </c>
       <c r="F6">
-        <v>500000</v>
-      </c>
-      <c r="H6" s="3"/>
+        <f t="shared" si="1"/>
+        <v>490000</v>
+      </c>
+      <c r="G6">
+        <v>12345</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>